<commit_message>
Added another test metagenome sample
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1605.4.metagenome.xlsx
+++ b/tests/fixtures/orderforms/1605.4.metagenome.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E4A34875-9329-5F45-926B-A1882957DA47}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A232511-177D-3E4A-97D9-C67323446A9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="19780" windowWidth="49600" windowHeight="9020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28860" yWindow="4780" windowWidth="22300" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order form" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4887" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4898" uniqueCount="305">
   <si>
     <t>cust002</t>
   </si>
@@ -948,6 +948,15 @@
   <si>
     <t>best</t>
   </si>
+  <si>
+    <t>Trefyrasex</t>
+  </si>
+  <si>
+    <t>Tuben</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
 </sst>
 </file>
 
@@ -1845,8 +1854,8 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="143" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D17" zoomScale="143" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2416,7 +2425,7 @@
       <c r="AC15" s="47"/>
       <c r="AD15" s="47"/>
     </row>
-    <row r="16" spans="1:30" ht="12.75" hidden="1" customHeight="1">
+    <row r="16" spans="1:30" ht="12.75" customHeight="1">
       <c r="A16" s="49" t="s">
         <v>242</v>
       </c>
@@ -2450,7 +2459,7 @@
       <c r="AC16" s="47"/>
       <c r="AD16" s="47"/>
     </row>
-    <row r="17" spans="1:30" ht="40.5" hidden="1" customHeight="1">
+    <row r="17" spans="1:30" ht="40.5" customHeight="1">
       <c r="A17" s="50" t="s">
         <v>243</v>
       </c>
@@ -2534,7 +2543,7 @@
       </c>
       <c r="AD17" s="54"/>
     </row>
-    <row r="18" spans="1:30" ht="18.75" hidden="1" customHeight="1">
+    <row r="18" spans="1:30" ht="18.75" customHeight="1">
       <c r="A18" s="49" t="s">
         <v>269</v>
       </c>
@@ -2771,25 +2780,51 @@
       <c r="AD21" s="54"/>
     </row>
     <row r="22" spans="1:30" ht="12.75" customHeight="1">
-      <c r="A22" s="72"/>
-      <c r="B22" s="51"/>
+      <c r="A22" s="72" t="s">
+        <v>302</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>20</v>
+      </c>
       <c r="C22" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="73"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="51"/>
+      <c r="D22" s="73" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="51" t="s">
+        <v>27</v>
+      </c>
       <c r="J22" s="54"/>
-      <c r="K22" s="70"/>
+      <c r="K22" s="70" t="s">
+        <v>303</v>
+      </c>
       <c r="L22" s="9"/>
       <c r="M22" s="54"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="70"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="70"/>
+      <c r="N22" s="70">
+        <v>1</v>
+      </c>
+      <c r="O22" s="70">
+        <v>2</v>
+      </c>
+      <c r="P22" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" s="70" t="s">
+        <v>304</v>
+      </c>
       <c r="R22" s="54"/>
       <c r="S22" s="71" t="s">
         <v>12</v>
@@ -44430,7 +44465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O1:O9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>